<commit_message>
Changes for IIS Deploy and Business partner module
</commit_message>
<xml_diff>
--- a/Troy.Web/Troy.Web/App_Data/ExcelFiles/Manufacturer NEW3.xlsx
+++ b/Troy.Web/Troy.Web/App_Data/ExcelFiles/Manufacturer NEW3.xlsx
@@ -24,7 +24,7 @@
     <t>Manufacturer Name</t>
   </si>
   <si>
-    <t>sony123</t>
+    <t>Micromax</t>
   </si>
 </sst>
 </file>
@@ -930,7 +930,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
sapout table.bulk addition changes in manufacturer,product group,employee,business partner module
</commit_message>
<xml_diff>
--- a/Troy.Web/Troy.Web/App_Data/ExcelFiles/Manufacturer NEW3.xlsx
+++ b/Troy.Web/Troy.Web/App_Data/ExcelFiles/Manufacturer NEW3.xlsx
@@ -24,7 +24,7 @@
     <t>Manufacturer Name</t>
   </si>
   <si>
-    <t>Micromax</t>
+    <t>Micromax111</t>
   </si>
 </sst>
 </file>
@@ -930,7 +930,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>